<commit_message>
Add CEIUSSI 2023 conference
</commit_message>
<xml_diff>
--- a/EN/cv_data.xlsx
+++ b/EN/cv_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Personales\CV\Vitae\EN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\GitRepos\CV\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947D8F66-6502-4241-B67F-C67F815FC021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B6B0F2-E31D-4384-B639-D47FEE1AF290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="3" xr2:uid="{290816F3-7D4B-4B8F-9C7B-5F4DF68E0B88}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{290816F3-7D4B-4B8F-9C7B-5F4DF68E0B88}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
   <si>
     <t>Degree</t>
   </si>
@@ -285,6 +285,19 @@
   </si>
   <si>
     <t>Presentation: Honeybee workers display task-related and subspecific patterns in their cuticular hydrocarbon profiles</t>
+  </si>
+  <si>
+    <t>Presentation: The expression of elongases and desaturases shed light on the CHC plasticity of honey
+bees (\textit{Apis mellifera})</t>
+  </si>
+  <si>
+    <t>September 19 2023</t>
+  </si>
+  <si>
+    <t>7th meeting of the Central European Section of the IUSSE</t>
+  </si>
+  <si>
+    <t>Cluj-Napoca, Romania</t>
   </si>
 </sst>
 </file>
@@ -898,10 +911,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3A69DC-CBB4-4DE7-92CD-AAB32432F059}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,73 +941,87 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating data for CV
</commit_message>
<xml_diff>
--- a/EN/cv_data.xlsx
+++ b/EN/cv_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Daniel\GitRepos\CV\EN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Personales\CV\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B6B0F2-E31D-4384-B639-D47FEE1AF290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129865A2-7DEA-48CF-B9C2-93E695532F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="3" activeTab="3" xr2:uid="{290816F3-7D4B-4B8F-9C7B-5F4DF68E0B88}"/>
+    <workbookView xWindow="24528" yWindow="1536" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{290816F3-7D4B-4B8F-9C7B-5F4DF68E0B88}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
   <si>
     <t>Degree</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Biocentre, Faculty of Biology, Julius-Maximilians-Universität Würzburg</t>
   </si>
   <si>
-    <t>December 2020 - Present</t>
-  </si>
-  <si>
     <t>Activities: Extraction and GC-MS analysis of Cuticular hydrocarbons.</t>
   </si>
   <si>
@@ -212,9 +209,6 @@
     <t>Foreigners promotion, Konrad-Adenauer-Stiftung</t>
   </si>
   <si>
-    <t>January 2021 - Present</t>
-  </si>
-  <si>
     <t>September 2020 - Present</t>
   </si>
   <si>
@@ -225,9 +219,6 @@
   </si>
   <si>
     <t>MS Office: Good Knowledge (User)</t>
-  </si>
-  <si>
-    <t>R: Intermediate knowledge</t>
   </si>
   <si>
     <t>Python: Basic knowledge</t>
@@ -298,6 +289,27 @@
   </si>
   <si>
     <t>Cluj-Napoca, Romania</t>
+  </si>
+  <si>
+    <t>January 2021 - December 2023</t>
+  </si>
+  <si>
+    <t>R: Advanced knowledge</t>
+  </si>
+  <si>
+    <t>December 2020 - December 2023</t>
+  </si>
+  <si>
+    <t>Doctoral researcher</t>
+  </si>
+  <si>
+    <t>Zoo3 department, Biocentre, Faculty of Biology, Julius-Maximilians-Universität Würzburg</t>
+  </si>
+  <si>
+    <t>January 2024 - Present</t>
+  </si>
+  <si>
+    <t>Project: Function of Cuticular Hydrocarbons in Honey bees</t>
   </si>
 </sst>
 </file>
@@ -359,9 +371,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -399,7 +411,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -505,7 +517,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -647,7 +659,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -732,10 +744,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66E35B5B-3565-4A47-A4B1-166D13E4C39C}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,69 +772,86 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>87</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>23</v>
+        <v>84</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -864,27 +893,27 @@
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -892,13 +921,13 @@
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>14</v>
@@ -913,7 +942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3A69DC-CBB4-4DE7-92CD-AAB32432F059}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
@@ -943,83 +972,83 @@
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
@@ -1036,7 +1065,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1075,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1060,13 +1089,13 @@
     </row>
     <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1092,7 +1121,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1106,13 +1135,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -1120,13 +1149,13 @@
     </row>
     <row r="3" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -1142,7 +1171,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,59 +1181,59 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add IUSSI 2024 congress
</commit_message>
<xml_diff>
--- a/EN/cv_data.xlsx
+++ b/EN/cv_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Personales\CV\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F0C4AC6-2827-4B25-BD86-81E07D3CB713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDBC61A-4444-4346-913B-4F0073E3916C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" activeTab="6" xr2:uid="{290816F3-7D4B-4B8F-9C7B-5F4DF68E0B88}"/>
+    <workbookView xWindow="10095" yWindow="0" windowWidth="10410" windowHeight="10905" firstSheet="3" activeTab="3" xr2:uid="{290816F3-7D4B-4B8F-9C7B-5F4DF68E0B88}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="93">
   <si>
     <t>Degree</t>
   </si>
@@ -310,6 +310,19 @@
   </si>
   <si>
     <t>Symposium of Communication and Chemical Ecology, 9th European Congress of Apidology</t>
+  </si>
+  <si>
+    <t>Honey bee (\textit{Apis mellifera}) CHC variations: New insight from desaturases and elongases
+expression assays</t>
+  </si>
+  <si>
+    <t>July 8 2024</t>
+  </si>
+  <si>
+    <t>European meeting of the International Union for the Study of Social Insects (IUSSI)</t>
+  </si>
+  <si>
+    <t>Lausanne, Switzerland</t>
   </si>
 </sst>
 </file>
@@ -940,10 +953,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3A69DC-CBB4-4DE7-92CD-AAB32432F059}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="43.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,85 +985,99 @@
     </row>
     <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1170,7 +1197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2DD866E-39D5-4EBE-807C-DFE0FC2C48E9}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>